<commit_message>
Regular vacation - forms fill changes.
</commit_message>
<xml_diff>
--- a/forms/regularDynamicVacationForm_academic.xlsx
+++ b/forms/regularDynamicVacationForm_academic.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/booogie-man-07/IdeaProjects/chatbot/forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25B5752-9665-F04A-B229-C9158C0443B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C271FCC2-86B4-024C-A932-10B3697C4459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
   <si>
     <t>Генеральному директору ООО "Гринхаус" Шилову Г.Ю.</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t>Непосредственный руководитель:</t>
-  </si>
-  <si>
-    <t>Генеральный директор</t>
-  </si>
-  <si>
-    <t>Г.Ю.Шилов</t>
   </si>
   <si>
     <t>(ФИО)</t>
@@ -210,72 +204,72 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -571,7 +565,7 @@
   <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection sqref="A1:E46"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.25" defaultRowHeight="11.5" customHeight="1"/>
@@ -585,270 +579,270 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
     </row>
     <row r="2" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A2" s="7"/>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="4"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
     </row>
     <row r="3" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A3" s="7"/>
-      <c r="B3" s="8"/>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="A3" s="4"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
     </row>
     <row r="4" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
     </row>
     <row r="5" spans="1:5" ht="19" customHeight="1">
-      <c r="A5" s="7"/>
-      <c r="B5" s="8"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9" t="s">
+      <c r="A5" s="4"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="19" customHeight="1">
-      <c r="A6" s="7"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="4"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
     </row>
     <row r="7" spans="1:5" ht="19" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="10" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>19</v>
+      <c r="E7" s="17" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="19" customHeight="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="12"/>
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:5" ht="14">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
       <c r="E9" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="5" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="19" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="14" t="s">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="14"/>
+      <c r="E11" s="21"/>
     </row>
     <row r="12" spans="1:5" ht="13">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4" t="s">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="22"/>
     </row>
     <row r="13" spans="1:5" ht="5" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5" ht="18" customHeight="1">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="E14" s="14"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="21"/>
     </row>
     <row r="15" spans="1:5" ht="13">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="4" t="s">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="22"/>
     </row>
     <row r="16" spans="1:5" ht="13">
-      <c r="A16" s="7"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5" ht="18" customHeight="1">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
     </row>
     <row r="18" spans="1:5" ht="19" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="16" t="s">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A19" s="7"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
     </row>
     <row r="20" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8"/>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
     </row>
     <row r="21" spans="1:5" ht="13">
-      <c r="A21" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21" s="9"/>
-      <c r="C21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
+      <c r="A21" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="16"/>
+      <c r="C21" s="16"/>
+      <c r="D21" s="16"/>
+      <c r="E21" s="16"/>
     </row>
     <row r="22" spans="1:5" ht="8" customHeight="1">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8"/>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
     </row>
     <row r="23" spans="1:5" ht="8" customHeight="1">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" ht="40" customHeight="1">
-      <c r="A24" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="9" t="s">
+      <c r="A24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C24" s="16"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+    </row>
+    <row r="25" spans="1:5" ht="13" customHeight="1">
+      <c r="A25" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+    </row>
+    <row r="26" spans="1:5" ht="22" customHeight="1">
+      <c r="A26" s="4"/>
+      <c r="B26" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="16"/>
+      <c r="E26" s="16"/>
+    </row>
+    <row r="27" spans="1:5" ht="13" customHeight="1">
+      <c r="A27" s="4"/>
+      <c r="B27" s="10"/>
+      <c r="C27" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="9"/>
-      <c r="E24" s="9"/>
-    </row>
-    <row r="25" spans="1:5" ht="13" customHeight="1">
-      <c r="A25" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-    </row>
-    <row r="26" spans="1:5" ht="22" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="13">
+      <c r="A28" s="5"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+    </row>
+    <row r="29" spans="1:5" ht="29" customHeight="1">
+      <c r="A29" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
-    </row>
-    <row r="27" spans="1:5" ht="13" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" s="19"/>
-      <c r="C27" s="18" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D27" s="18"/>
-      <c r="E27" s="18"/>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="13">
-      <c r="A28" s="8"/>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-    </row>
-    <row r="29" spans="1:5" ht="29" customHeight="1">
-      <c r="A29" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="21"/>
-      <c r="C29" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="20"/>
-      <c r="E29" s="22" t="s">
+      <c r="D29" s="11"/>
+      <c r="E29" s="12" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="13">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="20" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="17" t="s">
+      <c r="B30" s="20"/>
+      <c r="C30" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="23"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="13"/>
     </row>
     <row r="31" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
+      <c r="A31" s="4"/>
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
     </row>
     <row r="32" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8"/>
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="A32" s="4"/>
+      <c r="B32" s="5"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
     </row>
     <row r="33" spans="1:5" ht="13">
       <c r="A33" s="24" t="s">
@@ -856,8 +850,8 @@
       </c>
       <c r="B33" s="24"/>
       <c r="C33" s="24"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="11"/>
     </row>
     <row r="34" spans="1:5" ht="13">
       <c r="A34" s="24" t="s">
@@ -865,115 +859,111 @@
       </c>
       <c r="B34" s="24"/>
       <c r="C34" s="24"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="11"/>
     </row>
     <row r="35" spans="1:5" ht="18" customHeight="1">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="1:5" ht="13" customHeight="1">
+      <c r="A36" s="23" t="s">
+        <v>2</v>
+      </c>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="25" t="s">
+    </row>
+    <row r="37" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A37" s="15"/>
+      <c r="B37" s="11"/>
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="11"/>
+    </row>
+    <row r="38" spans="1:5" ht="18" customHeight="1">
+      <c r="A38" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" spans="1:5" ht="14">
+      <c r="A39" s="23" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="13" customHeight="1">
-      <c r="A36" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A37" s="26"/>
-      <c r="B37" s="20"/>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-    </row>
-    <row r="38" spans="1:5" ht="18" customHeight="1">
-      <c r="A38" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="25"/>
-    </row>
-    <row r="39" spans="1:5" ht="14">
-      <c r="A39" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="20"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="11"/>
       <c r="E39" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="18" customHeight="1">
-      <c r="A40" s="26"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
+      <c r="A40" s="15"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="11"/>
     </row>
     <row r="41" spans="1:5" ht="13">
       <c r="A41" s="24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B41" s="24"/>
       <c r="C41" s="24"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
     </row>
     <row r="42" spans="1:5" ht="13">
-      <c r="A42" s="26"/>
+      <c r="A42" s="15"/>
       <c r="B42" s="27"/>
       <c r="C42" s="27"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="25"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="14"/>
     </row>
     <row r="43" spans="1:5" ht="14">
-      <c r="A43" s="26"/>
-      <c r="B43" s="6" t="s">
+      <c r="A43" s="15"/>
+      <c r="B43" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="20"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="11"/>
       <c r="E43" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="44" spans="1:5" ht="11.5" customHeight="1">
-      <c r="A44" s="26"/>
-      <c r="B44" s="20"/>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="11"/>
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="11"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1">
-      <c r="A45" s="5" t="s">
+      <c r="A45" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="B45" s="5"/>
-      <c r="C45" s="5"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="25"/>
+      <c r="B45" s="23"/>
+      <c r="C45" s="23"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="14"/>
     </row>
     <row r="46" spans="1:5" ht="14">
-      <c r="A46" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B46" s="5"/>
-      <c r="C46" s="5"/>
-      <c r="D46" s="20"/>
+      <c r="A46" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="23"/>
+      <c r="C46" s="23"/>
+      <c r="D46" s="11"/>
       <c r="E46" s="3" t="s">
         <v>8</v>
       </c>
@@ -981,6 +971,19 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="25">
+    <mergeCell ref="A29:B29"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="A46:C46"/>
+    <mergeCell ref="A35:C35"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A39:C39"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A45:C45"/>
     <mergeCell ref="D5:E6"/>
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="D7:D8"/>
@@ -993,19 +996,6 @@
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A46:C46"/>
-    <mergeCell ref="A35:C35"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A45:C45"/>
-    <mergeCell ref="A29:B29"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B42:C42"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>